<commit_message>
Corrected clock for park hours that pass midnight
</commit_message>
<xml_diff>
--- a/Code/GUI Development Simulation.xlsx
+++ b/Code/GUI Development Simulation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -301,13 +301,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="13" style="0" width="4.71"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -354,7 +367,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>2000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,72 +393,84 @@
         <v>0.458333333333333</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H9" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L9" s="3" t="n">
         <v>0.625</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="J9" s="3" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="L9" s="3" t="n">
-        <v>0.708333333333333</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>10</v>
       </c>
       <c r="N9" s="3" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P9" s="3" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="R9" s="3" t="n">
         <v>0.75</v>
       </c>
-      <c r="O9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="S9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" s="3" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="Q9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="R9" s="3" t="n">
+      <c r="U9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="V9" s="3" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="S9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T9" s="3" t="n">
+      <c r="W9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" s="3" t="n">
         <v>0.875</v>
       </c>
-      <c r="U9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V9" s="3" t="n">
+      <c r="Y9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="3" t="n">
         <v>0.916666666666667</v>
       </c>
-      <c r="W9" s="1" t="n">
+      <c r="AA9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="3" t="n">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="AC9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="X9" s="3" t="n">
-        <v>0.958333333333333</v>
-      </c>
-      <c r="Y9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AA9" s="1" t="n">
+      <c r="AE9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -481,7 +506,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>14</v>
@@ -493,13 +518,13 @@
         <v>15</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>17</v>
@@ -532,11 +557,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.79"/>
   </cols>
@@ -584,7 +609,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -916,10 +941,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -998,7 +1023,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1021,7 +1046,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1044,7 +1069,7 @@
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>